<commit_message>
feat: vanilla buildings to js initial pass
</commit_message>
<xml_diff>
--- a/tools/buildings.xlsx
+++ b/tools/buildings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacke\Documents\Paradox Interactive\Victoria 3\mod\ARoAI\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC949EB9-0B43-475B-9777-E0750AE8E590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A88F70B-C296-4FC4-A868-C477EF8269AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FEBF1DC4-2923-4A95-AFAE-D20A21531141}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="10815" windowWidth="12000" windowHeight="5400" xr2:uid="{FEBF1DC4-2923-4A95-AFAE-D20A21531141}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,12 +324,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -344,9 +350,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -666,7 +675,7 @@
   <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,38 +720,38 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="b">
+      <c r="J2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: updated building list
</commit_message>
<xml_diff>
--- a/tools/buildings.xlsx
+++ b/tools/buildings.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacke\Documents\Paradox Interactive\Victoria 3\mod\ARoAI\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A88F70B-C296-4FC4-A868-C477EF8269AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D38E457-2BE1-455D-84D0-255D855DE746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="10815" windowWidth="12000" windowHeight="5400" xr2:uid="{FEBF1DC4-2923-4A95-AFAE-D20A21531141}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="5280" windowWidth="10920" windowHeight="10800" xr2:uid="{FEBF1DC4-2923-4A95-AFAE-D20A21531141}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="141">
   <si>
     <t>building_government_administration</t>
   </si>
@@ -50,9 +51,6 @@
     <t>dc</t>
   </si>
   <si>
-    <t>building_railway</t>
-  </si>
-  <si>
     <t>building_port</t>
   </si>
   <si>
@@ -134,12 +132,6 @@
     <t>building_food_industry</t>
   </si>
   <si>
-    <t>building_textile_mills</t>
-  </si>
-  <si>
-    <t>building_furniture_manufacturies</t>
-  </si>
-  <si>
     <t>building_glassworks</t>
   </si>
   <si>
@@ -152,9 +144,6 @@
     <t>building_shipyards</t>
   </si>
   <si>
-    <t>building_munition_plants</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -245,9 +234,6 @@
     <t>building_computer_manufactories</t>
   </si>
   <si>
-    <t>building_household_appliance_manufactories</t>
-  </si>
-  <si>
     <t>building_copper_mine</t>
   </si>
   <si>
@@ -309,13 +295,178 @@
   </si>
   <si>
     <t>building_electronics_manufactories</t>
+  </si>
+  <si>
+    <t>building_distilleries</t>
+  </si>
+  <si>
+    <t>building_textile_manufactories</t>
+  </si>
+  <si>
+    <t>building_furniture_manufactories</t>
+  </si>
+  <si>
+    <t>building_explosives_industry</t>
+  </si>
+  <si>
+    <t>building_consumer_electronics_manufactories</t>
+  </si>
+  <si>
+    <t>building_conscription_center</t>
+  </si>
+  <si>
+    <t>building_urban_center</t>
+  </si>
+  <si>
+    <t>building_slums</t>
+  </si>
+  <si>
+    <t>building_nuclear_research_facility</t>
+  </si>
+  <si>
+    <t>building_military_research_facility</t>
+  </si>
+  <si>
+    <t>building_humanities_research_facility</t>
+  </si>
+  <si>
+    <t>building_science_research_facility</t>
+  </si>
+  <si>
+    <t>building_eiffel_tower</t>
+  </si>
+  <si>
+    <t>building_angkor_wat</t>
+  </si>
+  <si>
+    <t>building_big_ben</t>
+  </si>
+  <si>
+    <t>building_forbidden_city</t>
+  </si>
+  <si>
+    <t>building_hagia_sophia</t>
+  </si>
+  <si>
+    <t>building_saint_basils_cathedral</t>
+  </si>
+  <si>
+    <t>building_statue_of_liberty</t>
+  </si>
+  <si>
+    <t>building_taj_mahal</t>
+  </si>
+  <si>
+    <t>building_vatican_city</t>
+  </si>
+  <si>
+    <t>building_white_house</t>
+  </si>
+  <si>
+    <t>building_kremlin</t>
+  </si>
+  <si>
+    <t>building_national_mall</t>
+  </si>
+  <si>
+    <t>building_monte_carlo_casino</t>
+  </si>
+  <si>
+    <t>building_machu_picchu</t>
+  </si>
+  <si>
+    <t>building_argebam</t>
+  </si>
+  <si>
+    <t>building_chichen_itza</t>
+  </si>
+  <si>
+    <t>building_easter_island_heads</t>
+  </si>
+  <si>
+    <t>building_eye_of_sahara</t>
+  </si>
+  <si>
+    <t>building_giza_necropolis</t>
+  </si>
+  <si>
+    <t>building_khaju_bridge</t>
+  </si>
+  <si>
+    <t>building_petra</t>
+  </si>
+  <si>
+    <t>building_capitol_hill</t>
+  </si>
+  <si>
+    <t>building_central_park</t>
+  </si>
+  <si>
+    <t>building_conventional_oil_well</t>
+  </si>
+  <si>
+    <t>building_un_conventional_oil_well</t>
+  </si>
+  <si>
+    <t>building_offshore_oil_well</t>
+  </si>
+  <si>
+    <t>building_conventional_gas_well</t>
+  </si>
+  <si>
+    <t>building_un_conventional_gas_well</t>
+  </si>
+  <si>
+    <t>building_offshore_gas_well</t>
+  </si>
+  <si>
+    <t>building_suez_canal</t>
+  </si>
+  <si>
+    <t>building_panama_canal</t>
+  </si>
+  <si>
+    <t>building_south_shore_canal</t>
+  </si>
+  <si>
+    <t>building_beauharnois_canal</t>
+  </si>
+  <si>
+    <t>building_wiley-dondero_canal</t>
+  </si>
+  <si>
+    <t>building_iroquois_canal</t>
+  </si>
+  <si>
+    <t>building_welland_canal</t>
+  </si>
+  <si>
+    <t>building_detroit_river</t>
+  </si>
+  <si>
+    <t>building_st_marys_canal</t>
+  </si>
+  <si>
+    <t>building_infrastructure</t>
+  </si>
+  <si>
+    <t>building_trade_center</t>
+  </si>
+  <si>
+    <t>building_skyscraper</t>
+  </si>
+  <si>
+    <t>building_housing</t>
+  </si>
+  <si>
+    <t>building_renewable_energy_facility</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,8 +474,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +509,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -347,22 +527,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -674,84 +889,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61956C1-F73F-4AFC-9587-99AB1262B269}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="74.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
+    </row>
+    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>4</v>
       </c>
-      <c r="J2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2" t="b">
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -827,7 +1042,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -862,7 +1077,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -897,7 +1112,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -932,7 +1147,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -967,7 +1182,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -1002,7 +1217,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1037,7 +1252,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1072,7 +1287,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1107,7 +1322,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1142,7 +1357,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -1177,7 +1392,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -1212,7 +1427,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -1247,7 +1462,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
@@ -1282,7 +1497,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
@@ -1317,7 +1532,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
@@ -1352,7 +1567,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
@@ -1387,7 +1602,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -1422,7 +1637,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
@@ -1457,7 +1672,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
@@ -1492,7 +1707,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
@@ -1527,7 +1742,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B25" s="1">
         <v>24</v>
@@ -1562,7 +1777,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
@@ -1597,7 +1812,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
@@ -1632,7 +1847,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" s="1">
         <v>27</v>
@@ -1667,7 +1882,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
@@ -1702,7 +1917,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1">
         <v>29</v>
@@ -1737,7 +1952,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1">
         <v>30</v>
@@ -1772,7 +1987,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="1">
         <v>31</v>
@@ -1807,7 +2022,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1">
         <v>32</v>
@@ -1842,7 +2057,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1">
         <v>33</v>
@@ -1877,7 +2092,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="1">
         <v>34</v>
@@ -1912,7 +2127,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1">
         <v>35</v>
@@ -1947,7 +2162,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="1">
         <v>36</v>
@@ -1982,7 +2197,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1">
         <v>37</v>
@@ -2017,7 +2232,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B39" s="1">
         <v>38</v>
@@ -2052,7 +2267,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" s="1">
         <v>39</v>
@@ -2087,7 +2302,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" s="1">
         <v>40</v>
@@ -2122,7 +2337,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" s="1">
         <v>41</v>
@@ -2157,7 +2372,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="1">
         <v>42</v>
@@ -2192,7 +2407,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" s="1">
         <v>43</v>
@@ -2227,7 +2442,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B45" s="1">
         <v>44</v>
@@ -2262,7 +2477,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="B46" s="1">
         <v>45</v>
@@ -2297,7 +2512,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B47" s="1">
         <v>46</v>
@@ -2332,7 +2547,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1">
         <v>47</v>
@@ -2367,7 +2582,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1">
         <v>48</v>
@@ -2402,7 +2617,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B50" s="1">
         <v>49</v>
@@ -2437,7 +2652,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1">
         <v>50</v>
@@ -2472,7 +2687,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1">
         <v>51</v>
@@ -2507,7 +2722,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1">
         <v>52</v>
@@ -2542,7 +2757,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B54" s="1">
         <v>53</v>
@@ -2577,7 +2792,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1">
         <v>54</v>
@@ -2612,7 +2827,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B56" s="1">
         <v>55</v>
@@ -2647,7 +2862,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1">
         <v>56</v>
@@ -2682,7 +2897,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B58" s="1">
         <v>57</v>
@@ -2717,7 +2932,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B59" s="1">
         <v>58</v>
@@ -2752,7 +2967,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B60" s="1">
         <v>59</v>
@@ -2787,7 +3002,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="B61" s="1">
         <v>60</v>
@@ -2822,10 +3037,10 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B62" s="1">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C62" s="1">
         <v>6</v>
@@ -2857,19 +3072,19 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B63" s="1">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C63" s="1">
         <v>6</v>
       </c>
-      <c r="D63" s="1">
-        <v>58</v>
+      <c r="D63" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="E63" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F63" s="1">
         <v>5</v>
@@ -2892,19 +3107,19 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B64" s="1">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C64" s="1">
         <v>6</v>
       </c>
-      <c r="D64" s="1">
-        <v>58</v>
+      <c r="D64" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="E64" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F64" s="1">
         <v>5</v>
@@ -2927,10 +3142,10 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B65" s="1">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C65" s="1">
         <v>6</v>
@@ -2939,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F65" s="1">
         <v>5</v>
@@ -2962,10 +3177,10 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B66" s="1">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C66" s="1">
         <v>6</v>
@@ -2974,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" s="1">
         <v>5</v>
@@ -2997,10 +3212,10 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B67" s="1">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C67" s="1">
         <v>6</v>
@@ -3009,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F67" s="1">
         <v>5</v>
@@ -3032,10 +3247,10 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B68" s="1">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C68" s="1">
         <v>6</v>
@@ -3044,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F68" s="1">
         <v>5</v>
@@ -3067,10 +3282,10 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B69" s="1">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C69" s="1">
         <v>6</v>
@@ -3079,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="E69" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F69" s="1">
         <v>5</v>
@@ -3102,10 +3317,10 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B70" s="1">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C70" s="1">
         <v>6</v>
@@ -3114,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F70" s="1">
         <v>5</v>
@@ -3137,10 +3352,10 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B71" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C71" s="1">
         <v>6</v>
@@ -3172,10 +3387,10 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B72" s="1">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C72" s="1">
         <v>6</v>
@@ -3206,11 +3421,11 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>67</v>
+      <c r="A73" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="B73" s="1">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C73" s="1">
         <v>6</v>
@@ -3219,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F73" s="1">
         <v>5</v>
@@ -3242,10 +3457,10 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B74" s="1">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1">
         <v>6</v>
@@ -3254,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="E74" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F74" s="1">
         <v>5</v>
@@ -3277,19 +3492,19 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B75" s="1">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C75" s="1">
         <v>6</v>
       </c>
-      <c r="D75" s="1" t="b">
-        <v>0</v>
+      <c r="D75" s="1">
+        <v>13</v>
       </c>
       <c r="E75" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F75" s="1">
         <v>5</v>
@@ -3312,10 +3527,10 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B76" s="1">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C76" s="1">
         <v>6</v>
@@ -3324,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F76" s="1">
         <v>5</v>
@@ -3347,16 +3562,16 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B77" s="1">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C77" s="1">
         <v>6</v>
       </c>
-      <c r="D77" s="1">
-        <v>13</v>
+      <c r="D77" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="E77" s="1">
         <v>15</v>
@@ -3382,10 +3597,10 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B78" s="1">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C78" s="1">
         <v>6</v>
@@ -3399,7 +3614,7 @@
       <c r="F78" s="1">
         <v>5</v>
       </c>
-      <c r="G78" s="1" t="s">
+      <c r="G78" s="1">
         <v>3</v>
       </c>
       <c r="H78" s="1" t="b">
@@ -3417,10 +3632,10 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="B79" s="1">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C79" s="1">
         <v>6</v>
@@ -3429,10 +3644,10 @@
         <v>0</v>
       </c>
       <c r="E79" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F79" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>3</v>
@@ -3452,10 +3667,10 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B80" s="1">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1">
         <v>6</v>
@@ -3464,28 +3679,1179 @@
         <v>0</v>
       </c>
       <c r="E80" s="1">
+        <v>14</v>
+      </c>
+      <c r="F80" s="1">
+        <v>5</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H80" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J80" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K80" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751FCB1A-8E05-4BE5-A8DB-737987BBF83C}">
+  <dimension ref="A1:B126"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>Sheet1!A2</f>
+        <v>building_government_administration</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>Sheet1!A3</f>
+        <v>building_university</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>Sheet1!A4</f>
+        <v>building_construction_sector</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>Sheet1!A5</f>
+        <v>building_infrastructure</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>Sheet1!A6</f>
+        <v>building_port</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>Sheet1!A7</f>
+        <v>building_barracks</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>Sheet1!A8</f>
+        <v>building_naval_base</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f>Sheet1!A9</f>
+        <v>building_nuclear_weapons_facility</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>Sheet1!A10</f>
+        <v>building_chemical_weapons_facility</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f>Sheet1!A11</f>
+        <v>building_biological_weapons_facility</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>Sheet1!A12</f>
+        <v>building_spaceport</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>Sheet1!A13</f>
+        <v>building_mission_control</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f>Sheet1!A14</f>
+        <v>building_airport</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>Sheet1!A15</f>
+        <v>building_logging_camp</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f>Sheet1!A16</f>
+        <v>building_fishing_wharf</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f>Sheet1!A17</f>
+        <v>building_rubber_plantation</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f>Sheet1!A18</f>
+        <v>building_oil_rig</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f>Sheet1!A19</f>
+        <v>building_natural_gas_well</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f>Sheet1!A20</f>
+        <v>building_coal_mine</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f>Sheet1!A21</f>
+        <v>building_iron_mine</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f>Sheet1!A22</f>
+        <v>building_copper_mine</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f>Sheet1!A23</f>
+        <v>building_rare_earth_elements_mine</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f>Sheet1!A24</f>
+        <v>building_lead_mine</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f>Sheet1!A25</f>
+        <v>building_bauxite_mine</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f>Sheet1!A26</f>
+        <v>building_uranium_mine</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f>Sheet1!A27</f>
+        <v>building_phosphorus_mine</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f>Sheet1!A28</f>
+        <v>building_gold_mine</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f>Sheet1!A29</f>
+        <v>building_rye_farm</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f>Sheet1!A30</f>
+        <v>building_wheat_farm</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f>Sheet1!A31</f>
+        <v>building_rice_farm</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f>Sheet1!A32</f>
+        <v>building_maize_farm</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f>Sheet1!A33</f>
+        <v>building_millet_farm</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f>Sheet1!A34</f>
+        <v>building_livestock_ranch</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f>Sheet1!A35</f>
+        <v>building_cotton_plantation</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f>Sheet1!A36</f>
+        <v>building_dye_plantation</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f>Sheet1!A37</f>
+        <v>building_silk_plantation</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f>Sheet1!A38</f>
+        <v>building_banana_plantation</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f>Sheet1!A39</f>
+        <v>building_sugar_plantation</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f>Sheet1!A40</f>
+        <v>building_tea_plantation</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>Sheet1!A41</f>
+        <v>building_coffee_plantation</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f>Sheet1!A42</f>
+        <v>building_tobacco_plantation</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f>Sheet1!A43</f>
+        <v>building_opium_plantation</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f>Sheet1!A44</f>
+        <v>building_food_industry</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f>Sheet1!A45</f>
+        <v>building_textile_manufactories</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f>Sheet1!A46</f>
+        <v>building_furniture_manufactories</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f>Sheet1!A47</f>
+        <v>building_glassworks</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f>Sheet1!A48</f>
+        <v>building_tool_manufactories</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="str">
+        <f>Sheet1!A49</f>
+        <v>building_paper_manufactories</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <f>Sheet1!A50</f>
+        <v>building_chemical_plants</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f>Sheet1!A51</f>
+        <v>building_synthetics_plant</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f>Sheet1!A52</f>
+        <v>building_steelworks</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f>Sheet1!A53</f>
+        <v>building_aluminum_refinery</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f>Sheet1!A54</f>
+        <v>building_motor_industry</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f>Sheet1!A55</f>
+        <v>building_automobile_manufactories</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f>Sheet1!A56</f>
+        <v>building_shipyards</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f>Sheet1!A57</f>
+        <v>building_drydocks</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f>Sheet1!A58</f>
+        <v>building_electronics_manufactories</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f>Sheet1!A59</f>
+        <v>building_combustion_plant</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f>Sheet1!A60</f>
+        <v>building_nuclear_power_plant</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f>Sheet1!A61</f>
+        <v>building_renewable_energy_facility</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f>Sheet1!A62</f>
+        <v>building_geothermal_power_plant</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f>Sheet1!A63</f>
+        <v>building_small_arms_manufactories</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f>Sheet1!A64</f>
+        <v>building_explosives_industry</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f>Sheet1!A65</f>
+        <v>building_fuel_refineries</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f>Sheet1!A66</f>
+        <v>building_semiconductor_manufactories</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f>Sheet1!A67</f>
+        <v>building_advanced_military_manufactories</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f>Sheet1!A68</f>
+        <v>building_aircraft_manufactories</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f>Sheet1!A69</f>
+        <v>building_uranium_refineries</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f>Sheet1!A70</f>
+        <v>building_battery_manufactories</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f>Sheet1!A71</f>
+        <v>building_pharmaceutical_industry</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f>Sheet1!A72</f>
+        <v>building_computer_manufactories</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f>Sheet1!A73</f>
+        <v>building_consumer_electronics_manufactories</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f>Sheet1!A74</f>
+        <v>building_telecommunications</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f>Sheet1!A75</f>
+        <v>building_tourism_industry</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f>Sheet1!A76</f>
+        <v>building_financial_services</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f>Sheet1!A77</f>
+        <v>building_media_industry</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <f>Sheet1!A78</f>
+        <v>building_hospitals</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <f>Sheet1!A79</f>
+        <v>building_skyscraper</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <f>Sheet1!A80</f>
+        <v>building_distilleries</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82" s="1">
+        <f>Sheet1!A81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B83" s="1">
+        <f>Sheet1!A82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B84" s="1">
+        <f>Sheet1!A83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85" s="1">
+        <f>Sheet1!A84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" s="1">
+        <f>Sheet1!A85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" s="1">
+        <f>Sheet1!A86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B88" s="1">
+        <f>Sheet1!A87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B89" s="1">
+        <f>Sheet1!A88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" s="1">
+        <f>Sheet1!A89</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B91" s="1">
+        <f>Sheet1!A90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B92" s="1">
+        <f>Sheet1!A91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" s="1">
+        <f>Sheet1!A92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" s="1">
+        <f>Sheet1!A93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B95" s="1">
+        <f>Sheet1!A94</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="1">
+        <f>Sheet1!A95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B97" s="1">
+        <f>Sheet1!A96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="1">
+        <f>Sheet1!A97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" s="1">
+        <f>Sheet1!A98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F80" s="1">
-        <v>5</v>
-      </c>
-      <c r="G80" s="1">
-        <v>3</v>
-      </c>
-      <c r="H80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I80" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K80" s="1" t="b">
-        <v>1</v>
+      <c r="B100" s="1">
+        <f>Sheet1!A99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B101" s="1">
+        <f>Sheet1!A100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B102" s="1">
+        <f>Sheet1!A101</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B103" s="1">
+        <f>Sheet1!A102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B104" s="1">
+        <f>Sheet1!A103</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B105" s="1">
+        <f>Sheet1!A104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" s="1">
+        <f>Sheet1!A105</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B107" s="1">
+        <f>Sheet1!A106</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B108" s="1">
+        <f>Sheet1!A107</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B109" s="1">
+        <f>Sheet1!A108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B110" s="1">
+        <f>Sheet1!A109</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B111" s="1">
+        <f>Sheet1!A110</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B112" s="1">
+        <f>Sheet1!A111</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B113" s="1">
+        <f>Sheet1!A112</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B114" s="1">
+        <f>Sheet1!A113</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B115" s="1">
+        <f>Sheet1!A114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B116" s="1">
+        <f>Sheet1!A115</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B117" s="1">
+        <f>Sheet1!A116</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B118" s="1">
+        <f>Sheet1!A117</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B119" s="1">
+        <f>Sheet1!A118</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B120" s="1">
+        <f>Sheet1!A119</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B121" s="1">
+        <f>Sheet1!A120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="1">
+        <f>Sheet1!A121</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B123" s="1">
+        <f>Sheet1!A122</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B124" s="1">
+        <f>Sheet1!A123</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B125" s="1">
+        <f>Sheet1!A124</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B126" s="1">
+        <f>Sheet1!A125</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>